<commit_message>
update versi 561 ocp qa
</commit_message>
<xml_diff>
--- a/Daily Activity BSI/Daily Activities 16 Maret 2023.xlsx
+++ b/Daily Activity BSI/Daily Activities 16 Maret 2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSI SuperApp Rebranding\Daily Activity BSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AB9870-788D-49B6-8183-FEF790FFC776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EF981E-5A22-4837-B64F-F4C74AAE4BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12570" yWindow="15" windowWidth="16125" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Aktivitas</t>
   </si>
@@ -177,6 +177,51 @@
 6. Paket Data Tri Positive
 7. Paket Data Indosat Positive
 8. Gopay Positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. LinkAja Positive
+2. Tarik Tunai Tanpa Kartu Indomaret Negative
+3. Tarik Tunai Tanpa Kartu ATM BSI Negative
+4. Paket Data XL  Negative 
+5. Flow Favourite Transaction
+</t>
+  </si>
+  <si>
+    <t>1. Tarik Tunai Indomaret Positive
+2. Tarik Tunai ATM BSI Positive
+3. Link Aja Syariah Positive + Negative
+4. LinkAja Negative
+5. BPJS Ketenagakerjaan BPU Negative
+6. Kitabisa Positive + Negative
+7. List Recent Transaction Positive
+8. Universitas Ahmad Dahlan Positive + Negative
+9. Jadiberkah Positive Negative</t>
+  </si>
+  <si>
+    <t>Running SuperApp Rebrand</t>
+  </si>
+  <si>
+    <t>1. Pelaporan Transaksi
+2. Pelaporan Melalui Mutasi
+3. Akademik Bayar ID Positive + Negative</t>
+  </si>
+  <si>
+    <t>1. Rumah Zakat Indonesia Positive + Negative
+2. Pulsa Indosat Positive + Negative
+3. Paket Data Telkomsel Positive + Negative
+4. Paket Data Indosat Positive + Negative
+5. Pulsa XL Positive + Negative
+6. Pulsa Tri Positive</t>
+  </si>
+  <si>
+    <t>1. Pulsa Tri Negative
+2. Paket Data Telkomsel Positive + Negative
+3. Paket Data Tri Positive +Negative 
+4. Pulsa Smartfren Positive + Negative
+5. Pulsa Telkomsel Positive + Negative
+6. Dana Positive + Negative
+7. Gopay Positive + Negative
+8. Ovo Positive + Negative</t>
   </si>
 </sst>
 </file>
@@ -247,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -275,6 +320,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -617,14 +668,14 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="36.28515625" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -845,7 +896,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>45021</v>
       </c>
@@ -868,50 +919,120 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="1"/>
+    <row r="12" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>45026</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8">
+        <v>5</v>
+      </c>
+      <c r="D12" s="8">
+        <v>5</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>45027</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="8">
+        <v>12</v>
+      </c>
+      <c r="D13" s="8">
+        <v>12</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>45028</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="8">
+        <v>4</v>
+      </c>
+      <c r="D14" s="8">
+        <v>4</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>45029</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="8">
+        <v>13</v>
+      </c>
+      <c r="D15" s="8">
+        <v>13</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>45030</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="13">
+        <v>15</v>
+      </c>
+      <c r="D16" s="8">
+        <v>15</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>

</xml_diff>

<commit_message>
update terbaru 8 juni 2023
</commit_message>
<xml_diff>
--- a/Daily Activity BSI/Daily Activities 16 Maret 2023.xlsx
+++ b/Daily Activity BSI/Daily Activities 16 Maret 2023.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSI SuperApp Rebranding\Daily Activity BSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EF981E-5A22-4837-B64F-F4C74AAE4BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D7E772-A8AD-48D6-A071-B6F243772E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12570" yWindow="15" windowWidth="16125" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10170" yWindow="510" windowWidth="17865" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aktivitas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
   <si>
     <t>Aktivitas</t>
   </si>
@@ -223,12 +236,89 @@
 7. Gopay Positive + Negative
 8. Ovo Positive + Negative</t>
   </si>
+  <si>
+    <t>Running Regresi 1-10B</t>
+  </si>
+  <si>
+    <t>1. MPN Negative
+2. MPN DJA Positive
+3. MPN DJP Positive
+4. MPN DJBC Positive
+5. Aqiqah Wanita Off Positive
+6. Aqiqah Wanita On Positive
+7. Aqiqah Pria Off Positive
+8. Aqiqah Pria Off Negative
+9. ShopeePay Positive
+10. CAR Premi Reguler Positive
+11. CAR Tagihan Lainnya Positive</t>
+  </si>
+  <si>
+    <t>1. Takaful Positive
+2. CAR Tagihan Lainnya Negative
+3. Takaful Negative</t>
+  </si>
+  <si>
+    <t>Maintenance Script dan Upload Report</t>
+  </si>
+  <si>
+    <t>1. Pulsa Telkomsel Positive + Negative
+2. MPN Positive + Negative
+3. CAR Tagihan Lainnya Positive + Negative
+4. CAR Premi Reguler Positive + Negative</t>
+  </si>
+  <si>
+    <t>1. Aqiqah Pria Off Positive
+2. Aqiqah Wanita Off Positive
+3. Aqiqah Negative</t>
+  </si>
+  <si>
+    <t>1. Download Mutasi E-Statement
+2. Gopay
+3. BPJS Ketenagakerjaan BPU
+4. BPJS Ketenagakerjaan PU</t>
+  </si>
+  <si>
+    <t>Maintenance Script</t>
+  </si>
+  <si>
+    <t>1. MPN DJCB Positive 
+2. MPN DJCB Negative
+3. MPN DJP Positive</t>
+  </si>
+  <si>
+    <t>1. BPJS Ketenagakerjaan PU Positive + Negative 
+2. Social Media
+3. View List Recent Transaction Positive + Negative</t>
+  </si>
+  <si>
+    <t>1. ShopeePay Positive+Negative
+2. Pelaporan Melalui Mutasi
+3. LinkAja Positive+Negative</t>
+  </si>
+  <si>
+    <t>1. Pulsa Indosat Negative
+2. Pulsa Tri Positive + Negative
+3. Paket Data Indosat Positive</t>
+  </si>
+  <si>
+    <t>1. Change Profile Pic
+2. Kitabisa.id
+3. View List Recent Transaction Bayar Beli</t>
+  </si>
+  <si>
+    <t>1. Change Email Positive + Negative
+2. Social Media</t>
+  </si>
+  <si>
+    <t>1. Change Profile Pic 
+Note: Hanya bisa melakukan non transaksi tanpa pin</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,8 +334,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,6 +357,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -301,12 +403,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -318,14 +416,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -667,482 +774,654 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" ht="44.1" customHeight="1">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="345" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+    <row r="3" spans="1:7" ht="345">
+      <c r="A3" s="5">
         <v>45001</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="6">
         <v>13</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <v>7</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="6">
         <v>6</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+    <row r="4" spans="1:7" ht="240">
+      <c r="A4" s="5">
         <v>45002</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>13</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>13</v>
       </c>
-      <c r="E4" s="8">
-        <v>0</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+    <row r="5" spans="1:7" ht="135">
+      <c r="A5" s="5">
         <v>45005</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="6">
         <v>5</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <v>5</v>
       </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="9" t="s">
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+    <row r="6" spans="1:7" ht="165">
+      <c r="A6" s="5">
         <v>45006</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <v>9</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <v>9</v>
       </c>
-      <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="F6" s="9" t="s">
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+    <row r="7" spans="1:7" ht="90">
+      <c r="A7" s="8">
         <v>45009</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <v>6</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>6</v>
       </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+    <row r="8" spans="1:7" ht="90">
+      <c r="A8" s="5">
         <v>45012</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="6">
         <v>6</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <v>6</v>
       </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="9" t="s">
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+    <row r="9" spans="1:7" ht="135">
+      <c r="A9" s="5">
         <v>45015</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="6">
         <v>9</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="6">
         <v>9</v>
       </c>
-      <c r="E9" s="8">
-        <v>0</v>
-      </c>
-      <c r="F9" s="9" t="s">
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+    <row r="10" spans="1:7" ht="150">
+      <c r="A10" s="5">
         <v>45020</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="6">
         <v>8</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="6">
         <v>8</v>
       </c>
-      <c r="E10" s="8">
-        <v>0</v>
-      </c>
-      <c r="F10" s="9" t="s">
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+    <row r="11" spans="1:7" ht="120">
+      <c r="A11" s="5">
         <v>45021</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="6">
         <v>8</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="6">
         <v>8</v>
       </c>
-      <c r="E11" s="8">
-        <v>0</v>
-      </c>
-      <c r="F11" s="9" t="s">
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+    <row r="12" spans="1:7" ht="120">
+      <c r="A12" s="5">
         <v>45026</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="6">
         <v>5</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <v>5</v>
       </c>
-      <c r="E12" s="8">
-        <v>0</v>
-      </c>
-      <c r="F12" s="9" t="s">
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+    <row r="13" spans="1:7" ht="150">
+      <c r="A13" s="5">
         <v>45027</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="6">
         <v>12</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="6">
         <v>12</v>
       </c>
-      <c r="E13" s="8">
-        <v>0</v>
-      </c>
-      <c r="F13" s="9" t="s">
+      <c r="E13" s="6">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+    <row r="14" spans="1:7" ht="60">
+      <c r="A14" s="5">
         <v>45028</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="6">
         <v>4</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="6">
         <v>4</v>
       </c>
-      <c r="E14" s="8">
-        <v>0</v>
-      </c>
-      <c r="F14" s="9" t="s">
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+    <row r="15" spans="1:7" ht="135">
+      <c r="A15" s="5">
         <v>45029</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="6">
         <v>13</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="6">
         <v>13</v>
       </c>
-      <c r="E15" s="8">
-        <v>0</v>
-      </c>
-      <c r="F15" s="9" t="s">
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+    <row r="16" spans="1:7" ht="135">
+      <c r="A16" s="5">
         <v>45030</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="10">
         <v>15</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="6">
         <v>15</v>
       </c>
-      <c r="E16" s="8">
-        <v>0</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="12" t="s">
+      <c r="E16" s="6">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="165">
+      <c r="A17" s="5">
+        <v>45033</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="6">
+        <v>11</v>
+      </c>
+      <c r="D17" s="6">
+        <v>11</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="11.25" customHeight="1">
+      <c r="A18" s="5">
+        <v>45034</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="6">
+        <v>3</v>
+      </c>
+      <c r="D18" s="6">
+        <v>3</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="60">
+      <c r="A19" s="5">
+        <v>45043</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="6">
+        <v>4</v>
+      </c>
+      <c r="D19" s="6">
+        <v>4</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45">
+      <c r="A20" s="5">
+        <v>45044</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="6">
+        <v>3</v>
+      </c>
+      <c r="D20" s="6">
+        <v>3</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="60">
+      <c r="A21" s="5">
+        <v>45048</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="6">
+        <v>4</v>
+      </c>
+      <c r="D21" s="6">
+        <v>4</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45">
+      <c r="A22" s="5">
+        <v>45049</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="6">
+        <v>3</v>
+      </c>
+      <c r="D22" s="6">
+        <v>3</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="75">
+      <c r="A23" s="5">
+        <v>45050</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="6">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6">
+        <f>C23</f>
+        <v>5</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="45">
+      <c r="A24" s="5">
+        <v>45051</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="6">
+        <v>5</v>
+      </c>
+      <c r="D24" s="6">
+        <f>C24</f>
+        <v>5</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="45">
+      <c r="A25" s="5">
+        <v>45054</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="6">
+        <v>4</v>
+      </c>
+      <c r="D25" s="6">
+        <f>C25</f>
+        <v>4</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45">
+      <c r="A26" s="5">
+        <v>45055</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="6">
+        <v>3</v>
+      </c>
+      <c r="D26" s="6">
+        <f>C26</f>
+        <v>3</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30">
+      <c r="A27" s="5">
+        <v>45056</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="6">
+        <v>3</v>
+      </c>
+      <c r="D27" s="6">
+        <v>3</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45">
+      <c r="A28" s="5">
+        <v>45076</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="6">
+        <v>1</v>
+      </c>
+      <c r="D28" s="6">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1151,7 +1430,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1160,7 +1439,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1169,7 +1448,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>

</xml_diff>

<commit_message>
backup sebelum standarisasi 22 juni 2023
</commit_message>
<xml_diff>
--- a/Daily Activity BSI/Daily Activities 16 Maret 2023.xlsx
+++ b/Daily Activity BSI/Daily Activities 16 Maret 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSI SuperApp Rebranding\Daily Activity BSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D7E772-A8AD-48D6-A071-B6F243772E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AB8437-2E17-438D-871D-78E87B098530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10170" yWindow="510" windowWidth="17865" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aktivitas" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="54">
   <si>
     <t>Aktivitas</t>
   </si>
@@ -46,9 +46,6 @@
   <si>
     <t>Status
 (Tercapai, Tdk Tercapai)</t>
-  </si>
-  <si>
-    <t>Nama</t>
   </si>
   <si>
     <t>Plan (Jumlah)</t>
@@ -313,12 +310,57 @@
     <t>1. Change Profile Pic 
 Note: Hanya bisa melakukan non transaksi tanpa pin</t>
   </si>
+  <si>
+    <t>1. Pajak/Cukai/SBN/Paspor Positive + Negative
+2. Tarik Tunai Gerai Indomaret Positive</t>
+  </si>
+  <si>
+    <t>1. Tarik Tunai Gerai Indomaret Negative 
+2. E-Wallet Paytren Positive + Negative</t>
+  </si>
+  <si>
+    <t>Maintenance Script SuperApp Rebrand</t>
+  </si>
+  <si>
+    <t>1. Pulsa Smartfren Positive + Negative
+2. Paket Data Indosat Positive + Negative</t>
+  </si>
+  <si>
+    <t>Harry Setiawan</t>
+  </si>
+  <si>
+    <t>1. Pulsa Smartfren Negative
+2. List Recent Transaction Bayar Beli</t>
+  </si>
+  <si>
+    <t>1. Pulsa Tri Negative
+2. Ewallet ShopeePay</t>
+  </si>
+  <si>
+    <t>1. Ewallet Ovo Negative
+2. Dompet Dhuafa Positive</t>
+  </si>
+  <si>
+    <t>1. Ewallet LinkAja Syariah Negative
+2. Ewallet LinkAja Syariah Positive</t>
+  </si>
+  <si>
+    <t>1. Ewallet Gopay Negative
+2. Ewallet Gopay Positive
+3. Change Email Negative</t>
+  </si>
+  <si>
+    <t>1.Mengikuti kegiatan workshop offline automation di APL Tower (Basic UFT One, ALM Legacy dan ALM Octain, Standarisasi Pembuatan Script BSI Mobile SuperAppa</t>
+  </si>
+  <si>
+    <t>Workshop Offline Automation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -431,8 +473,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -452,9 +503,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -492,9 +543,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -527,26 +578,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -579,26 +613,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -772,31 +789,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-    </row>
-    <row r="2" spans="1:7" ht="44.1" customHeight="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:7" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -804,13 +821,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>3</v>
@@ -819,12 +836,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="345">
+    <row r="3" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>45001</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6">
         <v>13</v>
@@ -836,18 +853,18 @@
         <v>6</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="240">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>45002</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="6">
         <v>13</v>
@@ -859,18 +876,18 @@
         <v>0</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="135">
+    </row>
+    <row r="5" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>45005</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6">
         <v>5</v>
@@ -882,18 +899,18 @@
         <v>0</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="165">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>45006</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="6">
         <v>9</v>
@@ -905,18 +922,18 @@
         <v>0</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="90">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>45009</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="6">
         <v>6</v>
@@ -928,18 +945,18 @@
         <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="90">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>45012</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="6">
         <v>6</v>
@@ -951,18 +968,18 @@
         <v>0</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="135">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>45015</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="6">
         <v>9</v>
@@ -974,18 +991,18 @@
         <v>0</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="150">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>45020</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="6">
         <v>8</v>
@@ -997,18 +1014,18 @@
         <v>0</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="120">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>45021</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="6">
         <v>8</v>
@@ -1020,18 +1037,18 @@
         <v>0</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="120">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>45026</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="6">
         <v>5</v>
@@ -1043,18 +1060,18 @@
         <v>0</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="150">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>45027</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="6">
         <v>12</v>
@@ -1066,18 +1083,18 @@
         <v>0</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="60">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>45028</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="6">
         <v>4</v>
@@ -1089,18 +1106,18 @@
         <v>0</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="135">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>45029</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="6">
         <v>13</v>
@@ -1112,18 +1129,18 @@
         <v>0</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="135">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>45030</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="10">
         <v>15</v>
@@ -1135,18 +1152,18 @@
         <v>0</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="165">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>45033</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="6">
         <v>11</v>
@@ -1158,18 +1175,18 @@
         <v>0</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="11.25" customHeight="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>45034</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="6">
         <v>3</v>
@@ -1181,18 +1198,18 @@
         <v>0</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="60">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>45043</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="6">
         <v>4</v>
@@ -1204,18 +1221,18 @@
         <v>0</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>45044</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="6">
         <v>3</v>
@@ -1227,18 +1244,18 @@
         <v>0</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="60">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>45048</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="6">
         <v>4</v>
@@ -1250,18 +1267,18 @@
         <v>0</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>45049</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="6">
         <v>3</v>
@@ -1273,18 +1290,18 @@
         <v>0</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="75">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>45050</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="6">
         <v>5</v>
@@ -1297,18 +1314,18 @@
         <v>0</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>45051</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="6">
         <v>5</v>
@@ -1321,18 +1338,18 @@
         <v>0</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>45054</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="6">
         <v>4</v>
@@ -1345,18 +1362,18 @@
         <v>0</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>45055</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="6">
         <v>3</v>
@@ -1369,18 +1386,18 @@
         <v>0</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>45056</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="6">
         <v>3</v>
@@ -1392,18 +1409,18 @@
         <v>0</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>45076</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="6">
         <v>1</v>
@@ -1415,47 +1432,225 @@
         <v>0</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>45084</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="1">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="1"/>
+    <row r="30" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>45085</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="1">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>45086</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4</v>
+      </c>
+      <c r="D31" s="1">
+        <f>C31</f>
+        <v>4</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>45089</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" ref="D32" si="0">C32</f>
+        <v>2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>45090</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="15">
+        <v>2</v>
+      </c>
+      <c r="D33" s="15">
+        <f t="shared" ref="D33" si="1">C33</f>
+        <v>2</v>
+      </c>
+      <c r="E33" s="15">
+        <v>0</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>45091</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="15">
+        <v>2</v>
+      </c>
+      <c r="D34" s="15">
+        <f>C34</f>
+        <v>2</v>
+      </c>
+      <c r="E34" s="15">
+        <v>0</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>45096</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="15">
+        <v>2</v>
+      </c>
+      <c r="D35" s="15">
+        <f t="shared" ref="D35:D36" si="2">C35</f>
+        <v>2</v>
+      </c>
+      <c r="E35" s="15">
+        <v>0</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>45097</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="15">
+        <v>3</v>
+      </c>
+      <c r="D36" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E36" s="15">
+        <v>0</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>45098</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="6">
+        <v>1</v>
+      </c>
+      <c r="D37" s="6">
+        <f t="shared" ref="D37" si="3">C37</f>
+        <v>1</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>